<commit_message>
do deep refactoring for SOLID
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdnguyen\Desktop\jira_confluence_automator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91CD7D2-C963-4A13-A645-F48E2FC8DF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B0E7C4-6FCE-48DA-9582-95085A5477F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <t>ConfluencePageURL</t>
   </si>
   <si>
-    <t>https://pfteamspace.pepperl-fuchs.com/x/oNfxGQ</t>
+    <t>https://pfteamspace.pepperl-fuchs.com/x/FOX3GQ</t>
   </si>
 </sst>
 </file>

</xml_diff>